<commit_message>
init, edit TemplateReport/Report-DSHS.xlsx, add phone
</commit_message>
<xml_diff>
--- a/VS_LOAN.Core.Web/App_Data/TemplateReport/Report-DSHS.xlsx
+++ b/VS_LOAN.Core.Web/App_Data/TemplateReport/Report-DSHS.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Data\Projects\C10\VS_LOAN\VS_LOAN.Core.Web\App_Data\TemplateReport\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Dev\my8\vs_loan_hung\VS_LOAN.Core.Web\App_Data\TemplateReport\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
   <si>
     <t>STT</t>
   </si>
@@ -69,6 +69,9 @@
   </si>
   <si>
     <t>Kết quả hồ sơ</t>
+  </si>
+  <si>
+    <t>Số điện thoại</t>
   </si>
 </sst>
 </file>
@@ -76,8 +79,8 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="2">
-    <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="164" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="164" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="165" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
   <fonts count="14" x14ac:knownFonts="1">
     <font>
@@ -344,7 +347,7 @@
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="43" fontId="11" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="164" fontId="11" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="82">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -407,10 +410,55 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="12" fillId="4" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="12" fillId="4" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -519,54 +567,9 @@
     <xf numFmtId="0" fontId="6" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
@@ -872,24 +875,27 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A3:P4"/>
+  <dimension ref="A3:Q4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H7" sqref="H7"/>
+      <selection activeCell="I8" sqref="I8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="4.33203125" style="26" customWidth="1"/>
-    <col min="2" max="7" width="8.88671875" style="26"/>
-    <col min="8" max="8" width="10.21875" style="26" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="13.6640625" style="26" bestFit="1" customWidth="1"/>
-    <col min="10" max="14" width="8.88671875" style="26"/>
-    <col min="15" max="15" width="11.33203125" style="26" bestFit="1" customWidth="1"/>
-    <col min="16" max="16384" width="8.88671875" style="26"/>
+    <col min="2" max="5" width="8.88671875" style="26"/>
+    <col min="6" max="6" width="12.77734375" style="26" customWidth="1"/>
+    <col min="7" max="7" width="15.33203125" style="26" customWidth="1"/>
+    <col min="8" max="8" width="8.88671875" style="26"/>
+    <col min="9" max="9" width="10.21875" style="26" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="13.6640625" style="26" bestFit="1" customWidth="1"/>
+    <col min="11" max="15" width="8.88671875" style="26"/>
+    <col min="16" max="16" width="11.33203125" style="26" bestFit="1" customWidth="1"/>
+    <col min="17" max="16384" width="8.88671875" style="26"/>
   </cols>
   <sheetData>
-    <row r="3" spans="1:16" s="25" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:17" s="25" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="23" t="s">
         <v>0</v>
       </c>
@@ -906,40 +912,43 @@
         <v>3</v>
       </c>
       <c r="F3" s="23" t="s">
+        <v>16</v>
+      </c>
+      <c r="G3" s="23" t="s">
         <v>4</v>
       </c>
-      <c r="G3" s="23" t="s">
+      <c r="H3" s="23" t="s">
         <v>5</v>
       </c>
-      <c r="H3" s="23" t="s">
+      <c r="I3" s="23" t="s">
         <v>15</v>
       </c>
-      <c r="I3" s="23" t="s">
+      <c r="J3" s="23" t="s">
         <v>6</v>
       </c>
-      <c r="J3" s="23" t="s">
+      <c r="K3" s="23" t="s">
         <v>7</v>
       </c>
-      <c r="K3" s="23" t="s">
+      <c r="L3" s="23" t="s">
         <v>8</v>
       </c>
-      <c r="L3" s="23" t="s">
+      <c r="M3" s="23" t="s">
         <v>10</v>
       </c>
-      <c r="M3" s="24" t="s">
+      <c r="N3" s="24" t="s">
         <v>11</v>
       </c>
-      <c r="N3" s="24" t="s">
+      <c r="O3" s="24" t="s">
         <v>12</v>
       </c>
-      <c r="O3" s="24" t="s">
+      <c r="P3" s="24" t="s">
         <v>13</v>
       </c>
-      <c r="P3" s="24" t="s">
+      <c r="Q3" s="24" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A4" s="27"/>
       <c r="B4" s="27"/>
       <c r="C4" s="27"/>
@@ -956,6 +965,7 @@
       <c r="N4" s="27"/>
       <c r="O4" s="27"/>
       <c r="P4" s="27"/>
+      <c r="Q4" s="27"/>
     </row>
   </sheetData>
   <phoneticPr fontId="9" type="noConversion"/>
@@ -976,85 +986,85 @@
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="20" spans="5:30" x14ac:dyDescent="0.25">
-      <c r="E20" s="68"/>
-      <c r="F20" s="69"/>
-      <c r="G20" s="69"/>
-      <c r="H20" s="69"/>
-      <c r="I20" s="69"/>
-      <c r="J20" s="69"/>
-      <c r="K20" s="69"/>
-      <c r="L20" s="69"/>
-      <c r="M20" s="69"/>
-      <c r="N20" s="69"/>
-      <c r="O20" s="69"/>
-      <c r="P20" s="69"/>
-      <c r="Q20" s="69"/>
-      <c r="R20" s="69"/>
-      <c r="S20" s="69"/>
-      <c r="T20" s="69"/>
-      <c r="U20" s="69"/>
-      <c r="V20" s="69"/>
-      <c r="W20" s="69"/>
-      <c r="X20" s="69"/>
-      <c r="Y20" s="69"/>
-      <c r="Z20" s="69"/>
-      <c r="AA20" s="69"/>
-      <c r="AB20" s="69"/>
-      <c r="AC20" s="69"/>
-      <c r="AD20" s="69"/>
+      <c r="E20" s="37"/>
+      <c r="F20" s="38"/>
+      <c r="G20" s="38"/>
+      <c r="H20" s="38"/>
+      <c r="I20" s="38"/>
+      <c r="J20" s="38"/>
+      <c r="K20" s="38"/>
+      <c r="L20" s="38"/>
+      <c r="M20" s="38"/>
+      <c r="N20" s="38"/>
+      <c r="O20" s="38"/>
+      <c r="P20" s="38"/>
+      <c r="Q20" s="38"/>
+      <c r="R20" s="38"/>
+      <c r="S20" s="38"/>
+      <c r="T20" s="38"/>
+      <c r="U20" s="38"/>
+      <c r="V20" s="38"/>
+      <c r="W20" s="38"/>
+      <c r="X20" s="38"/>
+      <c r="Y20" s="38"/>
+      <c r="Z20" s="38"/>
+      <c r="AA20" s="38"/>
+      <c r="AB20" s="38"/>
+      <c r="AC20" s="38"/>
+      <c r="AD20" s="38"/>
     </row>
     <row r="21" spans="5:30" x14ac:dyDescent="0.25">
-      <c r="E21" s="70"/>
-      <c r="F21" s="70"/>
-      <c r="G21" s="70"/>
-      <c r="H21" s="70"/>
-      <c r="I21" s="70"/>
-      <c r="J21" s="70"/>
-      <c r="K21" s="70"/>
-      <c r="L21" s="70"/>
-      <c r="M21" s="70"/>
-      <c r="N21" s="70"/>
-      <c r="O21" s="70"/>
-      <c r="P21" s="70"/>
-      <c r="Q21" s="70"/>
-      <c r="R21" s="70"/>
-      <c r="S21" s="70"/>
-      <c r="T21" s="70"/>
-      <c r="U21" s="70"/>
-      <c r="V21" s="70"/>
-      <c r="W21" s="70"/>
-      <c r="X21" s="70"/>
-      <c r="Y21" s="71"/>
-      <c r="Z21" s="72"/>
-      <c r="AA21" s="72"/>
+      <c r="E21" s="39"/>
+      <c r="F21" s="39"/>
+      <c r="G21" s="39"/>
+      <c r="H21" s="39"/>
+      <c r="I21" s="39"/>
+      <c r="J21" s="39"/>
+      <c r="K21" s="39"/>
+      <c r="L21" s="39"/>
+      <c r="M21" s="39"/>
+      <c r="N21" s="39"/>
+      <c r="O21" s="39"/>
+      <c r="P21" s="39"/>
+      <c r="Q21" s="39"/>
+      <c r="R21" s="39"/>
+      <c r="S21" s="39"/>
+      <c r="T21" s="39"/>
+      <c r="U21" s="39"/>
+      <c r="V21" s="39"/>
+      <c r="W21" s="39"/>
+      <c r="X21" s="39"/>
+      <c r="Y21" s="40"/>
+      <c r="Z21" s="41"/>
+      <c r="AA21" s="41"/>
       <c r="AB21" s="1"/>
       <c r="AC21" s="1"/>
       <c r="AD21" s="1"/>
     </row>
     <row r="22" spans="5:30" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="E22" s="73"/>
-      <c r="F22" s="73"/>
-      <c r="G22" s="73"/>
-      <c r="H22" s="73"/>
-      <c r="I22" s="73"/>
-      <c r="J22" s="73"/>
-      <c r="K22" s="73"/>
-      <c r="L22" s="73"/>
-      <c r="M22" s="73"/>
-      <c r="N22" s="73"/>
-      <c r="O22" s="73"/>
-      <c r="P22" s="73"/>
-      <c r="Q22" s="73"/>
-      <c r="R22" s="73"/>
-      <c r="S22" s="73"/>
-      <c r="T22" s="73"/>
-      <c r="U22" s="73"/>
-      <c r="V22" s="73"/>
-      <c r="W22" s="73"/>
-      <c r="X22" s="73"/>
-      <c r="Y22" s="72"/>
-      <c r="Z22" s="72"/>
-      <c r="AA22" s="72"/>
+      <c r="E22" s="42"/>
+      <c r="F22" s="42"/>
+      <c r="G22" s="42"/>
+      <c r="H22" s="42"/>
+      <c r="I22" s="42"/>
+      <c r="J22" s="42"/>
+      <c r="K22" s="42"/>
+      <c r="L22" s="42"/>
+      <c r="M22" s="42"/>
+      <c r="N22" s="42"/>
+      <c r="O22" s="42"/>
+      <c r="P22" s="42"/>
+      <c r="Q22" s="42"/>
+      <c r="R22" s="42"/>
+      <c r="S22" s="42"/>
+      <c r="T22" s="42"/>
+      <c r="U22" s="42"/>
+      <c r="V22" s="42"/>
+      <c r="W22" s="42"/>
+      <c r="X22" s="42"/>
+      <c r="Y22" s="41"/>
+      <c r="Z22" s="41"/>
+      <c r="AA22" s="41"/>
       <c r="AB22" s="1"/>
       <c r="AC22" s="1"/>
       <c r="AD22" s="1"/>
@@ -1080,62 +1090,62 @@
       <c r="V23" s="2"/>
       <c r="W23" s="2"/>
       <c r="X23" s="2"/>
-      <c r="Y23" s="72"/>
-      <c r="Z23" s="72"/>
-      <c r="AA23" s="72"/>
+      <c r="Y23" s="41"/>
+      <c r="Z23" s="41"/>
+      <c r="AA23" s="41"/>
       <c r="AB23" s="1"/>
       <c r="AC23" s="1"/>
       <c r="AD23" s="1"/>
     </row>
     <row r="24" spans="5:30" x14ac:dyDescent="0.25">
-      <c r="E24" s="74"/>
-      <c r="F24" s="75"/>
-      <c r="G24" s="75"/>
-      <c r="H24" s="75"/>
-      <c r="I24" s="75"/>
-      <c r="J24" s="75"/>
-      <c r="K24" s="75"/>
-      <c r="L24" s="75"/>
-      <c r="M24" s="75"/>
-      <c r="N24" s="75"/>
-      <c r="O24" s="75"/>
-      <c r="P24" s="75"/>
-      <c r="Q24" s="75"/>
-      <c r="R24" s="75"/>
-      <c r="S24" s="75"/>
-      <c r="T24" s="75"/>
-      <c r="U24" s="75"/>
-      <c r="V24" s="75"/>
-      <c r="W24" s="75"/>
-      <c r="X24" s="75"/>
-      <c r="Y24" s="72"/>
-      <c r="Z24" s="72"/>
-      <c r="AA24" s="72"/>
+      <c r="E24" s="43"/>
+      <c r="F24" s="44"/>
+      <c r="G24" s="44"/>
+      <c r="H24" s="44"/>
+      <c r="I24" s="44"/>
+      <c r="J24" s="44"/>
+      <c r="K24" s="44"/>
+      <c r="L24" s="44"/>
+      <c r="M24" s="44"/>
+      <c r="N24" s="44"/>
+      <c r="O24" s="44"/>
+      <c r="P24" s="44"/>
+      <c r="Q24" s="44"/>
+      <c r="R24" s="44"/>
+      <c r="S24" s="44"/>
+      <c r="T24" s="44"/>
+      <c r="U24" s="44"/>
+      <c r="V24" s="44"/>
+      <c r="W24" s="44"/>
+      <c r="X24" s="44"/>
+      <c r="Y24" s="41"/>
+      <c r="Z24" s="41"/>
+      <c r="AA24" s="41"/>
       <c r="AB24" s="1"/>
       <c r="AC24" s="1"/>
       <c r="AD24" s="1"/>
     </row>
     <row r="25" spans="5:30" x14ac:dyDescent="0.25">
-      <c r="E25" s="77"/>
-      <c r="F25" s="77"/>
-      <c r="G25" s="77"/>
-      <c r="H25" s="77"/>
-      <c r="I25" s="77"/>
-      <c r="J25" s="77"/>
-      <c r="K25" s="77"/>
-      <c r="L25" s="77"/>
-      <c r="M25" s="77"/>
-      <c r="N25" s="77"/>
-      <c r="O25" s="77"/>
-      <c r="P25" s="77"/>
-      <c r="Q25" s="77"/>
-      <c r="R25" s="77"/>
-      <c r="S25" s="77"/>
-      <c r="T25" s="77"/>
-      <c r="U25" s="77"/>
-      <c r="V25" s="77"/>
-      <c r="W25" s="77"/>
-      <c r="X25" s="77"/>
+      <c r="E25" s="32"/>
+      <c r="F25" s="32"/>
+      <c r="G25" s="32"/>
+      <c r="H25" s="32"/>
+      <c r="I25" s="32"/>
+      <c r="J25" s="32"/>
+      <c r="K25" s="32"/>
+      <c r="L25" s="32"/>
+      <c r="M25" s="32"/>
+      <c r="N25" s="32"/>
+      <c r="O25" s="32"/>
+      <c r="P25" s="32"/>
+      <c r="Q25" s="32"/>
+      <c r="R25" s="32"/>
+      <c r="S25" s="32"/>
+      <c r="T25" s="32"/>
+      <c r="U25" s="32"/>
+      <c r="V25" s="32"/>
+      <c r="W25" s="32"/>
+      <c r="X25" s="32"/>
       <c r="Y25" s="1"/>
       <c r="Z25" s="1"/>
       <c r="AA25" s="1"/>
@@ -1144,164 +1154,164 @@
       <c r="AD25" s="1"/>
     </row>
     <row r="26" spans="5:30" x14ac:dyDescent="0.25">
-      <c r="E26" s="77"/>
-      <c r="F26" s="77"/>
-      <c r="G26" s="77"/>
-      <c r="H26" s="77"/>
-      <c r="I26" s="77"/>
-      <c r="J26" s="77"/>
-      <c r="K26" s="77"/>
-      <c r="L26" s="77"/>
-      <c r="M26" s="77"/>
-      <c r="N26" s="77"/>
-      <c r="O26" s="77"/>
-      <c r="P26" s="77"/>
-      <c r="Q26" s="77"/>
-      <c r="R26" s="77"/>
-      <c r="S26" s="77"/>
-      <c r="T26" s="77"/>
-      <c r="U26" s="77"/>
-      <c r="V26" s="77"/>
-      <c r="W26" s="77"/>
-      <c r="X26" s="77"/>
+      <c r="E26" s="32"/>
+      <c r="F26" s="32"/>
+      <c r="G26" s="32"/>
+      <c r="H26" s="32"/>
+      <c r="I26" s="32"/>
+      <c r="J26" s="32"/>
+      <c r="K26" s="32"/>
+      <c r="L26" s="32"/>
+      <c r="M26" s="32"/>
+      <c r="N26" s="32"/>
+      <c r="O26" s="32"/>
+      <c r="P26" s="32"/>
+      <c r="Q26" s="32"/>
+      <c r="R26" s="32"/>
+      <c r="S26" s="32"/>
+      <c r="T26" s="32"/>
+      <c r="U26" s="32"/>
+      <c r="V26" s="32"/>
+      <c r="W26" s="32"/>
+      <c r="X26" s="32"/>
       <c r="Y26" s="3"/>
       <c r="Z26" s="3"/>
       <c r="AA26" s="3"/>
     </row>
     <row r="27" spans="5:30" x14ac:dyDescent="0.25">
-      <c r="E27" s="77"/>
-      <c r="F27" s="77"/>
-      <c r="G27" s="77"/>
-      <c r="H27" s="77"/>
-      <c r="I27" s="77"/>
-      <c r="J27" s="77"/>
-      <c r="K27" s="77"/>
-      <c r="L27" s="77"/>
-      <c r="M27" s="77"/>
-      <c r="N27" s="77"/>
-      <c r="O27" s="77"/>
-      <c r="P27" s="77"/>
-      <c r="Q27" s="77"/>
-      <c r="R27" s="77"/>
-      <c r="S27" s="77"/>
-      <c r="T27" s="77"/>
-      <c r="U27" s="77"/>
-      <c r="V27" s="77"/>
-      <c r="W27" s="77"/>
-      <c r="X27" s="77"/>
+      <c r="E27" s="32"/>
+      <c r="F27" s="32"/>
+      <c r="G27" s="32"/>
+      <c r="H27" s="32"/>
+      <c r="I27" s="32"/>
+      <c r="J27" s="32"/>
+      <c r="K27" s="32"/>
+      <c r="L27" s="32"/>
+      <c r="M27" s="32"/>
+      <c r="N27" s="32"/>
+      <c r="O27" s="32"/>
+      <c r="P27" s="32"/>
+      <c r="Q27" s="32"/>
+      <c r="R27" s="32"/>
+      <c r="S27" s="32"/>
+      <c r="T27" s="32"/>
+      <c r="U27" s="32"/>
+      <c r="V27" s="32"/>
+      <c r="W27" s="32"/>
+      <c r="X27" s="32"/>
       <c r="Y27" s="3"/>
       <c r="Z27" s="3"/>
       <c r="AA27" s="3"/>
     </row>
     <row r="28" spans="5:30" x14ac:dyDescent="0.25">
-      <c r="E28" s="78"/>
-      <c r="F28" s="78"/>
-      <c r="G28" s="78"/>
-      <c r="H28" s="78"/>
-      <c r="I28" s="78"/>
-      <c r="J28" s="78"/>
-      <c r="K28" s="78"/>
-      <c r="L28" s="78"/>
-      <c r="M28" s="78"/>
-      <c r="N28" s="78"/>
-      <c r="O28" s="78"/>
-      <c r="P28" s="78"/>
-      <c r="Q28" s="78"/>
-      <c r="R28" s="78"/>
-      <c r="S28" s="78"/>
-      <c r="T28" s="78"/>
-      <c r="U28" s="78"/>
-      <c r="V28" s="78"/>
-      <c r="W28" s="78"/>
-      <c r="X28" s="78"/>
-      <c r="Y28" s="78"/>
-      <c r="Z28" s="78"/>
-      <c r="AA28" s="78"/>
-      <c r="AB28" s="78"/>
-      <c r="AC28" s="78"/>
-      <c r="AD28" s="78"/>
+      <c r="E28" s="33"/>
+      <c r="F28" s="33"/>
+      <c r="G28" s="33"/>
+      <c r="H28" s="33"/>
+      <c r="I28" s="33"/>
+      <c r="J28" s="33"/>
+      <c r="K28" s="33"/>
+      <c r="L28" s="33"/>
+      <c r="M28" s="33"/>
+      <c r="N28" s="33"/>
+      <c r="O28" s="33"/>
+      <c r="P28" s="33"/>
+      <c r="Q28" s="33"/>
+      <c r="R28" s="33"/>
+      <c r="S28" s="33"/>
+      <c r="T28" s="33"/>
+      <c r="U28" s="33"/>
+      <c r="V28" s="33"/>
+      <c r="W28" s="33"/>
+      <c r="X28" s="33"/>
+      <c r="Y28" s="33"/>
+      <c r="Z28" s="33"/>
+      <c r="AA28" s="33"/>
+      <c r="AB28" s="33"/>
+      <c r="AC28" s="33"/>
+      <c r="AD28" s="33"/>
     </row>
     <row r="29" spans="5:30" x14ac:dyDescent="0.25">
-      <c r="E29" s="79"/>
-      <c r="F29" s="80"/>
-      <c r="G29" s="80"/>
-      <c r="H29" s="80"/>
-      <c r="I29" s="80"/>
-      <c r="J29" s="81"/>
-      <c r="K29" s="81"/>
-      <c r="L29" s="81"/>
-      <c r="M29" s="81"/>
-      <c r="N29" s="59"/>
-      <c r="O29" s="60"/>
-      <c r="P29" s="61"/>
-      <c r="Q29" s="61"/>
-      <c r="R29" s="61"/>
-      <c r="S29" s="61"/>
-      <c r="T29" s="61"/>
-      <c r="U29" s="61"/>
-      <c r="V29" s="61"/>
-      <c r="W29" s="61"/>
-      <c r="X29" s="62"/>
-      <c r="Y29" s="32"/>
-      <c r="Z29" s="33"/>
-      <c r="AA29" s="34"/>
+      <c r="E29" s="34"/>
+      <c r="F29" s="35"/>
+      <c r="G29" s="35"/>
+      <c r="H29" s="35"/>
+      <c r="I29" s="35"/>
+      <c r="J29" s="36"/>
+      <c r="K29" s="36"/>
+      <c r="L29" s="36"/>
+      <c r="M29" s="36"/>
+      <c r="N29" s="76"/>
+      <c r="O29" s="77"/>
+      <c r="P29" s="78"/>
+      <c r="Q29" s="78"/>
+      <c r="R29" s="78"/>
+      <c r="S29" s="78"/>
+      <c r="T29" s="78"/>
+      <c r="U29" s="78"/>
+      <c r="V29" s="78"/>
+      <c r="W29" s="78"/>
+      <c r="X29" s="79"/>
+      <c r="Y29" s="49"/>
+      <c r="Z29" s="50"/>
+      <c r="AA29" s="51"/>
     </row>
     <row r="30" spans="5:30" x14ac:dyDescent="0.25">
-      <c r="E30" s="79"/>
-      <c r="F30" s="79"/>
-      <c r="G30" s="79"/>
-      <c r="H30" s="79"/>
-      <c r="I30" s="41"/>
-      <c r="J30" s="44"/>
-      <c r="K30" s="45"/>
-      <c r="L30" s="44"/>
-      <c r="M30" s="45"/>
-      <c r="N30" s="46"/>
-      <c r="O30" s="47"/>
-      <c r="P30" s="48"/>
-      <c r="Q30" s="52"/>
-      <c r="R30" s="53"/>
-      <c r="S30" s="53"/>
-      <c r="T30" s="53"/>
-      <c r="U30" s="53"/>
-      <c r="V30" s="53"/>
-      <c r="W30" s="53"/>
-      <c r="X30" s="54"/>
-      <c r="Y30" s="35"/>
-      <c r="Z30" s="36"/>
-      <c r="AA30" s="37"/>
+      <c r="E30" s="34"/>
+      <c r="F30" s="34"/>
+      <c r="G30" s="34"/>
+      <c r="H30" s="34"/>
+      <c r="I30" s="58"/>
+      <c r="J30" s="61"/>
+      <c r="K30" s="62"/>
+      <c r="L30" s="61"/>
+      <c r="M30" s="62"/>
+      <c r="N30" s="63"/>
+      <c r="O30" s="64"/>
+      <c r="P30" s="65"/>
+      <c r="Q30" s="69"/>
+      <c r="R30" s="70"/>
+      <c r="S30" s="70"/>
+      <c r="T30" s="70"/>
+      <c r="U30" s="70"/>
+      <c r="V30" s="70"/>
+      <c r="W30" s="70"/>
+      <c r="X30" s="71"/>
+      <c r="Y30" s="52"/>
+      <c r="Z30" s="53"/>
+      <c r="AA30" s="54"/>
     </row>
     <row r="31" spans="5:30" x14ac:dyDescent="0.25">
-      <c r="E31" s="79"/>
-      <c r="F31" s="79"/>
-      <c r="G31" s="79"/>
-      <c r="H31" s="79"/>
-      <c r="I31" s="42"/>
-      <c r="J31" s="38"/>
-      <c r="K31" s="40"/>
-      <c r="L31" s="38"/>
-      <c r="M31" s="40"/>
-      <c r="N31" s="49"/>
-      <c r="O31" s="50"/>
-      <c r="P31" s="51"/>
-      <c r="Q31" s="55"/>
-      <c r="R31" s="56"/>
-      <c r="S31" s="63"/>
-      <c r="T31" s="63"/>
-      <c r="U31" s="63"/>
-      <c r="V31" s="63"/>
-      <c r="W31" s="63"/>
-      <c r="X31" s="63"/>
-      <c r="Y31" s="38"/>
-      <c r="Z31" s="39"/>
-      <c r="AA31" s="40"/>
+      <c r="E31" s="34"/>
+      <c r="F31" s="34"/>
+      <c r="G31" s="34"/>
+      <c r="H31" s="34"/>
+      <c r="I31" s="59"/>
+      <c r="J31" s="55"/>
+      <c r="K31" s="57"/>
+      <c r="L31" s="55"/>
+      <c r="M31" s="57"/>
+      <c r="N31" s="66"/>
+      <c r="O31" s="67"/>
+      <c r="P31" s="68"/>
+      <c r="Q31" s="72"/>
+      <c r="R31" s="73"/>
+      <c r="S31" s="80"/>
+      <c r="T31" s="80"/>
+      <c r="U31" s="80"/>
+      <c r="V31" s="80"/>
+      <c r="W31" s="80"/>
+      <c r="X31" s="80"/>
+      <c r="Y31" s="55"/>
+      <c r="Z31" s="56"/>
+      <c r="AA31" s="57"/>
     </row>
     <row r="32" spans="5:30" x14ac:dyDescent="0.25">
-      <c r="E32" s="79"/>
-      <c r="F32" s="79"/>
-      <c r="G32" s="79"/>
-      <c r="H32" s="79"/>
-      <c r="I32" s="43"/>
+      <c r="E32" s="34"/>
+      <c r="F32" s="34"/>
+      <c r="G32" s="34"/>
+      <c r="H32" s="34"/>
+      <c r="I32" s="60"/>
       <c r="J32" s="5"/>
       <c r="K32" s="5"/>
       <c r="L32" s="5"/>
@@ -1309,8 +1319,8 @@
       <c r="N32" s="12"/>
       <c r="O32" s="12"/>
       <c r="P32" s="12"/>
-      <c r="Q32" s="57"/>
-      <c r="R32" s="58"/>
+      <c r="Q32" s="74"/>
+      <c r="R32" s="75"/>
       <c r="S32" s="16"/>
       <c r="T32" s="15"/>
       <c r="U32" s="16"/>
@@ -1334,8 +1344,8 @@
       <c r="N33" s="13"/>
       <c r="O33" s="13"/>
       <c r="P33" s="13"/>
-      <c r="Q33" s="66"/>
-      <c r="R33" s="67"/>
+      <c r="Q33" s="81"/>
+      <c r="R33" s="29"/>
       <c r="S33" s="17"/>
       <c r="T33" s="17"/>
       <c r="U33" s="17"/>
@@ -1359,8 +1369,8 @@
       <c r="N34" s="20"/>
       <c r="O34" s="20"/>
       <c r="P34" s="20"/>
-      <c r="Q34" s="76"/>
-      <c r="R34" s="67"/>
+      <c r="Q34" s="28"/>
+      <c r="R34" s="29"/>
       <c r="S34" s="21"/>
       <c r="T34" s="22"/>
       <c r="U34" s="21"/>
@@ -1387,8 +1397,8 @@
       <c r="N35" s="14"/>
       <c r="O35" s="14"/>
       <c r="P35" s="14"/>
-      <c r="Q35" s="64"/>
-      <c r="R35" s="65"/>
+      <c r="Q35" s="30"/>
+      <c r="R35" s="31"/>
       <c r="S35" s="18"/>
       <c r="T35" s="18"/>
       <c r="U35" s="18"/>
@@ -1415,8 +1425,8 @@
       <c r="N36" s="14"/>
       <c r="O36" s="14"/>
       <c r="P36" s="14"/>
-      <c r="Q36" s="64"/>
-      <c r="R36" s="65"/>
+      <c r="Q36" s="30"/>
+      <c r="R36" s="31"/>
       <c r="S36" s="18"/>
       <c r="T36" s="18"/>
       <c r="U36" s="18"/>
@@ -1443,8 +1453,8 @@
       <c r="N37" s="14"/>
       <c r="O37" s="14"/>
       <c r="P37" s="14"/>
-      <c r="Q37" s="64"/>
-      <c r="R37" s="65"/>
+      <c r="Q37" s="30"/>
+      <c r="R37" s="31"/>
       <c r="S37" s="18"/>
       <c r="T37" s="18"/>
       <c r="U37" s="18"/>
@@ -1459,41 +1469,41 @@
       <c r="AD37" s="4"/>
     </row>
     <row r="38" spans="5:30" x14ac:dyDescent="0.25">
-      <c r="E38" s="28"/>
-      <c r="F38" s="28"/>
-      <c r="G38" s="28"/>
-      <c r="H38" s="28"/>
-      <c r="I38" s="28"/>
-      <c r="J38" s="28"/>
-      <c r="K38" s="28"/>
-      <c r="L38" s="28"/>
-      <c r="M38" s="28"/>
-      <c r="N38" s="28"/>
-      <c r="O38" s="28"/>
-      <c r="P38" s="28"/>
-      <c r="Q38" s="28"/>
-      <c r="R38" s="28"/>
-      <c r="S38" s="28"/>
-      <c r="T38" s="28"/>
-      <c r="U38" s="28"/>
-      <c r="V38" s="28"/>
-      <c r="W38" s="28"/>
-      <c r="X38" s="28"/>
-      <c r="Y38" s="28"/>
-      <c r="Z38" s="28"/>
-      <c r="AA38" s="28"/>
+      <c r="E38" s="45"/>
+      <c r="F38" s="45"/>
+      <c r="G38" s="45"/>
+      <c r="H38" s="45"/>
+      <c r="I38" s="45"/>
+      <c r="J38" s="45"/>
+      <c r="K38" s="45"/>
+      <c r="L38" s="45"/>
+      <c r="M38" s="45"/>
+      <c r="N38" s="45"/>
+      <c r="O38" s="45"/>
+      <c r="P38" s="45"/>
+      <c r="Q38" s="45"/>
+      <c r="R38" s="45"/>
+      <c r="S38" s="45"/>
+      <c r="T38" s="45"/>
+      <c r="U38" s="45"/>
+      <c r="V38" s="45"/>
+      <c r="W38" s="45"/>
+      <c r="X38" s="45"/>
+      <c r="Y38" s="45"/>
+      <c r="Z38" s="45"/>
+      <c r="AA38" s="45"/>
       <c r="AB38" s="4"/>
       <c r="AC38" s="4"/>
       <c r="AD38" s="4"/>
     </row>
     <row r="39" spans="5:30" x14ac:dyDescent="0.25">
-      <c r="E39" s="29"/>
-      <c r="F39" s="30"/>
-      <c r="G39" s="30"/>
-      <c r="H39" s="30"/>
-      <c r="I39" s="30"/>
-      <c r="J39" s="30"/>
-      <c r="K39" s="30"/>
+      <c r="E39" s="46"/>
+      <c r="F39" s="47"/>
+      <c r="G39" s="47"/>
+      <c r="H39" s="47"/>
+      <c r="I39" s="47"/>
+      <c r="J39" s="47"/>
+      <c r="K39" s="47"/>
       <c r="L39" s="10"/>
       <c r="M39" s="10"/>
       <c r="N39" s="10"/>
@@ -1501,38 +1511,21 @@
       <c r="P39" s="10"/>
       <c r="Q39" s="10"/>
       <c r="R39" s="10"/>
-      <c r="S39" s="31"/>
-      <c r="T39" s="31"/>
-      <c r="U39" s="31"/>
-      <c r="V39" s="31"/>
-      <c r="W39" s="31"/>
-      <c r="X39" s="31"/>
-      <c r="Y39" s="31"/>
-      <c r="Z39" s="31"/>
-      <c r="AA39" s="31"/>
+      <c r="S39" s="48"/>
+      <c r="T39" s="48"/>
+      <c r="U39" s="48"/>
+      <c r="V39" s="48"/>
+      <c r="W39" s="48"/>
+      <c r="X39" s="48"/>
+      <c r="Y39" s="48"/>
+      <c r="Z39" s="48"/>
+      <c r="AA39" s="48"/>
       <c r="AB39" s="4"/>
       <c r="AC39" s="4"/>
       <c r="AD39" s="4"/>
     </row>
   </sheetData>
   <mergeCells count="33">
-    <mergeCell ref="Q34:R34"/>
-    <mergeCell ref="Q35:R35"/>
-    <mergeCell ref="Q36:R36"/>
-    <mergeCell ref="E25:X25"/>
-    <mergeCell ref="E26:X26"/>
-    <mergeCell ref="E27:X27"/>
-    <mergeCell ref="E28:AD28"/>
-    <mergeCell ref="E29:E32"/>
-    <mergeCell ref="F29:F32"/>
-    <mergeCell ref="G29:G32"/>
-    <mergeCell ref="H29:H32"/>
-    <mergeCell ref="I29:M29"/>
-    <mergeCell ref="E20:AD20"/>
-    <mergeCell ref="E21:X21"/>
-    <mergeCell ref="Y21:AA24"/>
-    <mergeCell ref="E22:X22"/>
-    <mergeCell ref="E24:X24"/>
     <mergeCell ref="E38:AA38"/>
     <mergeCell ref="E39:K39"/>
     <mergeCell ref="S39:AA39"/>
@@ -1549,6 +1542,23 @@
     <mergeCell ref="W31:X31"/>
     <mergeCell ref="Q37:R37"/>
     <mergeCell ref="Q33:R33"/>
+    <mergeCell ref="E20:AD20"/>
+    <mergeCell ref="E21:X21"/>
+    <mergeCell ref="Y21:AA24"/>
+    <mergeCell ref="E22:X22"/>
+    <mergeCell ref="E24:X24"/>
+    <mergeCell ref="Q34:R34"/>
+    <mergeCell ref="Q35:R35"/>
+    <mergeCell ref="Q36:R36"/>
+    <mergeCell ref="E25:X25"/>
+    <mergeCell ref="E26:X26"/>
+    <mergeCell ref="E27:X27"/>
+    <mergeCell ref="E28:AD28"/>
+    <mergeCell ref="E29:E32"/>
+    <mergeCell ref="F29:F32"/>
+    <mergeCell ref="G29:G32"/>
+    <mergeCell ref="H29:H32"/>
+    <mergeCell ref="I29:M29"/>
   </mergeCells>
   <phoneticPr fontId="9" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>